<commit_message>
Version aktualisiert - "Antworten mischen" für SC Fragen hinzugefügt
</commit_message>
<xml_diff>
--- a/Vorlage (SC) - Import Excel-Datei in Datenbank.xlsx
+++ b/Vorlage (SC) - Import Excel-Datei in Datenbank.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="91">
   <si>
     <t>question_difficulty</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>SC-Test3</t>
+  </si>
+  <si>
+    <t>mix_answers</t>
   </si>
 </sst>
 </file>
@@ -326,7 +329,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -349,14 +352,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -661,15 +676,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BR3"/>
+  <dimension ref="A1:BS3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="BR9" sqref="BR9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -880,8 +895,11 @@
       <c r="BR1" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="BS1" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
@@ -996,8 +1014,11 @@
       <c r="BR2" s="2" t="s">
         <v>85</v>
       </c>
+      <c r="BS2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
@@ -1110,6 +1131,9 @@
       <c r="BP3" s="2"/>
       <c r="BQ3" s="2"/>
       <c r="BR3" s="2"/>
+      <c r="BS3">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>